<commit_message>
working through sept sweeps
</commit_message>
<xml_diff>
--- a/Raw Data/Arthropod_data.xlsx
+++ b/Raw Data/Arthropod_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11485" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11920" uniqueCount="508">
   <si>
     <t>location</t>
   </si>
@@ -1505,13 +1505,49 @@
     <t>Sept</t>
   </si>
   <si>
-    <t>Coal-S6-O1-SS-1</t>
+    <t>Pteromalidae?</t>
   </si>
   <si>
-    <t>Coal-S6-O1-SS-2</t>
+    <t>Eucera?</t>
   </si>
   <si>
-    <t>Pteromalidae?</t>
+    <t>CaS-Sept19-FF-1</t>
+  </si>
+  <si>
+    <t>CaS-Sept19-O5-SS-1</t>
+  </si>
+  <si>
+    <t>Coal-Sept-6-O1-SS-1</t>
+  </si>
+  <si>
+    <t>Coal-Sept-6-O1-SS-2</t>
+  </si>
+  <si>
+    <t>Curculionidae</t>
+  </si>
+  <si>
+    <t>SiCr-Sept-16-FF-1</t>
+  </si>
+  <si>
+    <t>white/black dots</t>
+  </si>
+  <si>
+    <t>Chrysomelidae?</t>
+  </si>
+  <si>
+    <t>IS - no gly</t>
+  </si>
+  <si>
+    <t>Oedipodinae?</t>
+  </si>
+  <si>
+    <t>Theriidae</t>
+  </si>
+  <si>
+    <t>spiderling</t>
+  </si>
+  <si>
+    <t>Eulophidae?</t>
   </si>
 </sst>
 </file>
@@ -1852,9 +1888,9 @@
   <dimension ref="A1:U1970"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1707" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1719" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="D1715" sqref="D1715:F1722"/>
+      <selection pane="bottomLeft" activeCell="C1781" sqref="C1781"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -57227,9 +57263,6 @@
       <c r="L1699" t="s">
         <v>99</v>
       </c>
-      <c r="P1699" t="s">
-        <v>135</v>
-      </c>
       <c r="Q1699" t="s">
         <v>102</v>
       </c>
@@ -57706,7 +57739,7 @@
         <v>1714</v>
       </c>
       <c r="B1713" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
       <c r="C1713" t="s">
         <v>70</v>
@@ -57750,7 +57783,7 @@
         <v>1715</v>
       </c>
       <c r="B1714" t="s">
-        <v>494</v>
+        <v>498</v>
       </c>
       <c r="C1714" t="s">
         <v>70</v>
@@ -58005,7 +58038,7 @@
         <v>75</v>
       </c>
       <c r="M1720" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="1721" spans="1:16" x14ac:dyDescent="0.35">
@@ -58082,348 +58115,2160 @@
       <c r="A1723">
         <v>1724</v>
       </c>
+      <c r="B1723" t="s">
+        <v>496</v>
+      </c>
+      <c r="C1723" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1723" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1723" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1723">
+        <v>19</v>
+      </c>
+      <c r="G1723" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1723" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1723">
+        <v>5</v>
+      </c>
+      <c r="J1723" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1723">
+        <v>1</v>
+      </c>
+      <c r="L1723" t="s">
+        <v>99</v>
+      </c>
+      <c r="M1723" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1723" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="1724" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1724">
         <v>1725</v>
       </c>
+      <c r="D1724" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1724" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1724">
+        <v>19</v>
+      </c>
+      <c r="G1724" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1724" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1724" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1724">
+        <v>2</v>
+      </c>
+      <c r="L1724" t="s">
+        <v>99</v>
+      </c>
+      <c r="M1724" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1724" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="1725" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1725">
         <v>1726</v>
       </c>
+      <c r="D1725" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1725" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1725">
+        <v>19</v>
+      </c>
+      <c r="G1725" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1725" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1725" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1725">
+        <v>1</v>
+      </c>
+      <c r="L1725" t="s">
+        <v>99</v>
+      </c>
+      <c r="M1725" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1725" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="1726" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1726">
         <v>1727</v>
       </c>
+      <c r="B1726" t="s">
+        <v>495</v>
+      </c>
+      <c r="D1726" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1726" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1726">
+        <v>19</v>
+      </c>
+      <c r="G1726" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1726" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1726" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1726">
+        <v>1</v>
+      </c>
+      <c r="L1726" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1726" t="s">
+        <v>288</v>
+      </c>
+      <c r="P1726" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="1727" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1727">
         <v>1728</v>
       </c>
+      <c r="D1727" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1727" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1727">
+        <v>19</v>
+      </c>
+      <c r="G1727" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1727" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1727">
+        <v>10</v>
+      </c>
+      <c r="J1727" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1727">
+        <v>1</v>
+      </c>
+      <c r="L1727" t="s">
+        <v>99</v>
+      </c>
+      <c r="M1727" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1727" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="1728" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1728">
         <v>1729</v>
       </c>
-    </row>
-    <row r="1729" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1728" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1728" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1728">
+        <v>19</v>
+      </c>
+      <c r="G1728" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1728" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1728">
+        <v>2</v>
+      </c>
+      <c r="J1728" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1728">
+        <v>1</v>
+      </c>
+      <c r="L1728" t="s">
+        <v>99</v>
+      </c>
+      <c r="M1728" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1728" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="1729" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1729">
         <v>1730</v>
       </c>
-    </row>
-    <row r="1730" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1729" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1729" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1729">
+        <v>19</v>
+      </c>
+      <c r="G1729" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1729" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1729">
+        <v>2</v>
+      </c>
+      <c r="J1729" t="s">
+        <v>380</v>
+      </c>
+      <c r="K1729">
+        <v>1</v>
+      </c>
+      <c r="L1729" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1729" t="s">
+        <v>145</v>
+      </c>
+      <c r="P1729" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q1729" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="1730" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1730">
         <v>1731</v>
       </c>
-    </row>
-    <row r="1731" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1730" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1730" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1730">
+        <v>19</v>
+      </c>
+      <c r="G1730" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1730" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1730">
+        <v>7</v>
+      </c>
+      <c r="J1730" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1730">
+        <v>1</v>
+      </c>
+      <c r="L1730" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1730" t="s">
+        <v>80</v>
+      </c>
+      <c r="P1730" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="1731" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1731">
         <v>1732</v>
       </c>
-    </row>
-    <row r="1732" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1731" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1731" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1731">
+        <v>19</v>
+      </c>
+      <c r="G1731" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1731" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1731">
+        <v>3</v>
+      </c>
+      <c r="J1731" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1731">
+        <v>1</v>
+      </c>
+      <c r="L1731" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1731" t="s">
+        <v>77</v>
+      </c>
+      <c r="P1731" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="1732" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1732">
         <v>1733</v>
       </c>
-    </row>
-    <row r="1733" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1732" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1732" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1732">
+        <v>19</v>
+      </c>
+      <c r="G1732" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1732" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1732">
+        <v>6</v>
+      </c>
+      <c r="J1732" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1732">
+        <v>1</v>
+      </c>
+      <c r="L1732" t="s">
+        <v>148</v>
+      </c>
+      <c r="M1732" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="1733" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1733">
         <v>1734</v>
       </c>
-    </row>
-    <row r="1734" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1733" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1733" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1733">
+        <v>19</v>
+      </c>
+      <c r="G1733" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1733" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1733">
+        <v>5</v>
+      </c>
+      <c r="J1733" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1733">
+        <v>1</v>
+      </c>
+      <c r="L1733" t="s">
+        <v>134</v>
+      </c>
+      <c r="M1733" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="1734" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1734">
         <v>1735</v>
       </c>
-    </row>
-    <row r="1735" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1734" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1734" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1734">
+        <v>19</v>
+      </c>
+      <c r="G1734" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1734" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1734">
+        <v>5</v>
+      </c>
+      <c r="J1734" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1734">
+        <v>1</v>
+      </c>
+      <c r="L1734" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1734" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="1735" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1735">
         <v>1736</v>
       </c>
-    </row>
-    <row r="1736" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1735" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1735" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1735">
+        <v>19</v>
+      </c>
+      <c r="G1735" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1735" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1735">
+        <v>10</v>
+      </c>
+      <c r="J1735" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1735">
+        <v>1</v>
+      </c>
+      <c r="L1735" t="s">
+        <v>148</v>
+      </c>
+      <c r="M1735" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="1736" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1736">
         <v>1737</v>
       </c>
-    </row>
-    <row r="1737" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1736" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1736" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1736">
+        <v>19</v>
+      </c>
+      <c r="G1736" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1736" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1736">
+        <v>8</v>
+      </c>
+      <c r="J1736" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1736">
+        <v>12</v>
+      </c>
+      <c r="L1736" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1736" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="1737" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1737">
         <v>1738</v>
       </c>
-    </row>
-    <row r="1738" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1737" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1737" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1737">
+        <v>19</v>
+      </c>
+      <c r="G1737" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1737" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1737">
+        <v>8</v>
+      </c>
+      <c r="J1737" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1737">
+        <v>1</v>
+      </c>
+      <c r="L1737" t="s">
+        <v>134</v>
+      </c>
+      <c r="M1737" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="1738" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1738">
         <v>1739</v>
       </c>
-    </row>
-    <row r="1739" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1738" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1738" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1738">
+        <v>19</v>
+      </c>
+      <c r="G1738" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1738" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1738">
+        <v>8</v>
+      </c>
+      <c r="J1738" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1738">
+        <v>1</v>
+      </c>
+      <c r="L1738" t="s">
+        <v>148</v>
+      </c>
+      <c r="M1738" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="1739" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1739">
         <v>1740</v>
       </c>
-    </row>
-    <row r="1740" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1739" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1739" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1739">
+        <v>19</v>
+      </c>
+      <c r="G1739" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1739" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1739">
+        <v>7</v>
+      </c>
+      <c r="J1739" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1739">
+        <v>2</v>
+      </c>
+      <c r="L1739" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1740" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1740">
         <v>1741</v>
       </c>
-    </row>
-    <row r="1741" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1740" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1740" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1740">
+        <v>19</v>
+      </c>
+      <c r="G1740" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1740" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1740">
+        <v>7</v>
+      </c>
+      <c r="J1740" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1740">
+        <v>2</v>
+      </c>
+      <c r="L1740" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1740" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="1741" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1741">
         <v>1742</v>
       </c>
-    </row>
-    <row r="1742" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1741" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1741" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1741">
+        <v>19</v>
+      </c>
+      <c r="G1741" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1741" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1741">
+        <v>7</v>
+      </c>
+      <c r="J1741" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1741">
+        <v>1</v>
+      </c>
+      <c r="L1741" t="s">
+        <v>148</v>
+      </c>
+      <c r="M1741" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="1742" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1742">
         <v>1743</v>
       </c>
-    </row>
-    <row r="1743" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1742" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1742" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1742">
+        <v>19</v>
+      </c>
+      <c r="G1742" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1742" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1742">
+        <v>9</v>
+      </c>
+      <c r="J1742" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1742">
+        <v>1</v>
+      </c>
+      <c r="L1742" t="s">
+        <v>99</v>
+      </c>
+      <c r="M1742" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1742" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="1743" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1743">
         <v>1744</v>
       </c>
-    </row>
-    <row r="1744" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1743" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1743" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1743">
+        <v>19</v>
+      </c>
+      <c r="G1743" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1743" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1743">
+        <v>9</v>
+      </c>
+      <c r="J1743" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1743">
+        <v>3</v>
+      </c>
+      <c r="L1743" t="s">
+        <v>148</v>
+      </c>
+      <c r="M1743" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="1744" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1744">
         <v>1745</v>
       </c>
-    </row>
-    <row r="1745" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1744" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1744" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1744">
+        <v>14</v>
+      </c>
+      <c r="H1744" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1744" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1744">
+        <v>1</v>
+      </c>
+      <c r="L1744" t="s">
+        <v>134</v>
+      </c>
+      <c r="M1744" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="1745" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1745">
         <v>1746</v>
       </c>
-    </row>
-    <row r="1746" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B1745" t="s">
+        <v>500</v>
+      </c>
+      <c r="C1745" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1745" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1745" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1745">
+        <v>14</v>
+      </c>
+      <c r="H1745" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1745" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1745">
+        <v>1</v>
+      </c>
+      <c r="L1745" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1745" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="1746" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1746">
         <v>1747</v>
       </c>
-    </row>
-    <row r="1747" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1746" t="s">
+        <v>265</v>
+      </c>
+      <c r="E1746" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1746">
+        <v>18</v>
+      </c>
+      <c r="G1746" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1746" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1746">
+        <v>10</v>
+      </c>
+      <c r="J1746" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1746">
+        <v>1</v>
+      </c>
+      <c r="L1746" t="s">
+        <v>148</v>
+      </c>
+      <c r="R1746" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="1747" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1747">
         <v>1748</v>
       </c>
-    </row>
-    <row r="1748" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1747" t="s">
+        <v>265</v>
+      </c>
+      <c r="E1747" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1747">
+        <v>18</v>
+      </c>
+      <c r="G1747" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1747" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1747">
+        <v>5</v>
+      </c>
+      <c r="J1747" t="s">
+        <v>380</v>
+      </c>
+      <c r="K1747">
+        <v>1</v>
+      </c>
+      <c r="L1747" t="s">
+        <v>148</v>
+      </c>
+      <c r="M1747" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="1748" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1748">
         <v>1749</v>
       </c>
-    </row>
-    <row r="1749" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1748" t="s">
+        <v>265</v>
+      </c>
+      <c r="E1748" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1748">
+        <v>18</v>
+      </c>
+      <c r="G1748" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1748" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1748">
+        <v>7</v>
+      </c>
+      <c r="J1748" t="s">
+        <v>380</v>
+      </c>
+      <c r="K1748">
+        <v>1</v>
+      </c>
+      <c r="L1748" t="s">
+        <v>148</v>
+      </c>
+      <c r="M1748" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="1749" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1749">
         <v>1750</v>
       </c>
-    </row>
-    <row r="1750" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1749" t="s">
+        <v>265</v>
+      </c>
+      <c r="E1749" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1749">
+        <v>18</v>
+      </c>
+      <c r="H1749" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1749" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1749">
+        <v>1</v>
+      </c>
+      <c r="L1749" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="1750" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1750">
         <v>1751</v>
       </c>
-    </row>
-    <row r="1751" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1750" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1750" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1750">
+        <v>23</v>
+      </c>
+      <c r="G1750" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1750" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1750">
+        <v>2</v>
+      </c>
+      <c r="J1750" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1750">
+        <v>4</v>
+      </c>
+      <c r="L1750" t="s">
+        <v>99</v>
+      </c>
+      <c r="M1750" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1750" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="1751" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1751">
         <v>1752</v>
       </c>
-    </row>
-    <row r="1752" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1751" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1751" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1751">
+        <v>23</v>
+      </c>
+      <c r="G1751" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1751" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1751" t="s">
+        <v>380</v>
+      </c>
+      <c r="K1751">
+        <v>1</v>
+      </c>
+      <c r="L1751" t="s">
+        <v>134</v>
+      </c>
+      <c r="R1751" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="1752" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1752">
         <v>1753</v>
       </c>
-    </row>
-    <row r="1753" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1752" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1752" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1752">
+        <v>23</v>
+      </c>
+      <c r="G1752" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1752" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1752" t="s">
+        <v>380</v>
+      </c>
+      <c r="K1752">
+        <v>1</v>
+      </c>
+      <c r="L1752" t="s">
+        <v>148</v>
+      </c>
+      <c r="M1752" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="1753" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1753">
         <v>1754</v>
       </c>
-    </row>
-    <row r="1754" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1753" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1753" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1753">
+        <v>23</v>
+      </c>
+      <c r="G1753" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1753" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1753" t="s">
+        <v>380</v>
+      </c>
+      <c r="K1753">
+        <v>1</v>
+      </c>
+      <c r="L1753" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1753" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="1754" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1754">
         <v>1755</v>
       </c>
-    </row>
-    <row r="1755" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1754" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1754" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1754">
+        <v>23</v>
+      </c>
+      <c r="G1754" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1754" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1754">
+        <v>9</v>
+      </c>
+      <c r="J1754" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1754">
+        <v>3</v>
+      </c>
+      <c r="L1754" t="s">
+        <v>99</v>
+      </c>
+      <c r="M1754" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1754" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="1755" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1755">
         <v>1756</v>
       </c>
-    </row>
-    <row r="1756" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1755" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1755" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1755">
+        <v>23</v>
+      </c>
+      <c r="G1755" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1755" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1755">
+        <v>9</v>
+      </c>
+      <c r="J1755" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1755">
+        <v>1</v>
+      </c>
+      <c r="L1755" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1755" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="1756" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1756">
         <v>1757</v>
       </c>
-    </row>
-    <row r="1757" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1756" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1756" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1756">
+        <v>23</v>
+      </c>
+      <c r="G1756" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1756" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1756">
+        <v>9</v>
+      </c>
+      <c r="J1756" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1756">
+        <v>2</v>
+      </c>
+      <c r="L1756" t="s">
+        <v>134</v>
+      </c>
+      <c r="R1756" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="1757" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1757">
         <v>1758</v>
       </c>
-    </row>
-    <row r="1758" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1757" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1757" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1757">
+        <v>23</v>
+      </c>
+      <c r="G1757" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1757" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1757">
+        <v>9</v>
+      </c>
+      <c r="J1757" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1757">
+        <v>1</v>
+      </c>
+      <c r="L1757" t="s">
+        <v>148</v>
+      </c>
+      <c r="M1757" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="1758" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1758">
         <v>1759</v>
       </c>
-    </row>
-    <row r="1759" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1758" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1758" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1758">
+        <v>23</v>
+      </c>
+      <c r="G1758" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1758" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1758">
+        <v>19</v>
+      </c>
+      <c r="J1758" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1758">
+        <v>4</v>
+      </c>
+      <c r="L1758" t="s">
+        <v>148</v>
+      </c>
+      <c r="M1758" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="1759" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1759">
         <v>1760</v>
       </c>
-    </row>
-    <row r="1760" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1759" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1759" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1759">
+        <v>23</v>
+      </c>
+      <c r="G1759" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1759" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1759">
+        <v>19</v>
+      </c>
+      <c r="J1759" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1759">
+        <v>1</v>
+      </c>
+      <c r="L1759" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1760" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1760">
         <v>1761</v>
       </c>
-    </row>
-    <row r="1761" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1760" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1760" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1760">
+        <v>23</v>
+      </c>
+      <c r="G1760" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1760" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1760">
+        <v>19</v>
+      </c>
+      <c r="J1760" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1760">
+        <v>1</v>
+      </c>
+      <c r="L1760" t="s">
+        <v>134</v>
+      </c>
+      <c r="M1760" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="1761" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1761">
         <v>1762</v>
       </c>
-    </row>
-    <row r="1762" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1761" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1761" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1761">
+        <v>23</v>
+      </c>
+      <c r="G1761" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1761" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1761">
+        <v>19</v>
+      </c>
+      <c r="J1761" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1761">
+        <v>1</v>
+      </c>
+      <c r="L1761" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1761" t="s">
+        <v>145</v>
+      </c>
+      <c r="P1761" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q1761" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="1762" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1762">
         <v>1763</v>
       </c>
-    </row>
-    <row r="1763" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1762" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1762" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1762">
+        <v>23</v>
+      </c>
+      <c r="G1762" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1762" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1762">
+        <v>5</v>
+      </c>
+      <c r="J1762" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1762">
+        <v>1</v>
+      </c>
+      <c r="L1762" t="s">
+        <v>99</v>
+      </c>
+      <c r="M1762" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1762" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="1763" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1763">
         <v>1764</v>
       </c>
-    </row>
-    <row r="1764" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1763" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1763" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1763">
+        <v>23</v>
+      </c>
+      <c r="G1763" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1763" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1763">
+        <v>1</v>
+      </c>
+      <c r="J1763" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1763">
+        <v>1</v>
+      </c>
+      <c r="L1763" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="1764" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1764">
         <v>1765</v>
       </c>
-    </row>
-    <row r="1765" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1764" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1764" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1764">
+        <v>23</v>
+      </c>
+      <c r="H1764" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1764" t="s">
+        <v>503</v>
+      </c>
+      <c r="K1764">
+        <v>1</v>
+      </c>
+      <c r="L1764" t="s">
+        <v>99</v>
+      </c>
+      <c r="M1764" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1764" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="1765" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1765">
         <v>1766</v>
       </c>
-    </row>
-    <row r="1766" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1765" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1765" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1765">
+        <v>23</v>
+      </c>
+      <c r="H1765" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1765" t="s">
+        <v>503</v>
+      </c>
+      <c r="K1765">
+        <v>2</v>
+      </c>
+      <c r="L1765" t="s">
+        <v>134</v>
+      </c>
+      <c r="M1765" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="1766" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1766">
         <v>1767</v>
       </c>
-    </row>
-    <row r="1767" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1766" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1766" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1766">
+        <v>23</v>
+      </c>
+      <c r="H1766" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1766" t="s">
+        <v>503</v>
+      </c>
+      <c r="K1766">
+        <v>1</v>
+      </c>
+      <c r="L1766" t="s">
+        <v>148</v>
+      </c>
+      <c r="M1766" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="1767" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1767">
         <v>1768</v>
       </c>
-    </row>
-    <row r="1768" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1767" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1767" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1767">
+        <v>23</v>
+      </c>
+      <c r="G1767" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1767" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1767">
+        <v>8</v>
+      </c>
+      <c r="J1767" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1767">
+        <v>1</v>
+      </c>
+      <c r="L1767" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1767" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="1768" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1768">
         <v>1769</v>
       </c>
-    </row>
-    <row r="1769" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1768" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1768" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1768">
+        <v>23</v>
+      </c>
+      <c r="G1768" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1768" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1768">
+        <v>8</v>
+      </c>
+      <c r="J1768" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1768">
+        <v>2</v>
+      </c>
+      <c r="L1768" t="s">
+        <v>99</v>
+      </c>
+      <c r="M1768" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1768" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="1769" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1769">
         <v>1770</v>
       </c>
-    </row>
-    <row r="1770" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1769" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1769" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1769">
+        <v>23</v>
+      </c>
+      <c r="G1769" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1769" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1769">
+        <v>7</v>
+      </c>
+      <c r="J1769" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1769">
+        <v>1</v>
+      </c>
+      <c r="L1769" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1769" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="1770" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1770">
         <v>1771</v>
       </c>
-    </row>
-    <row r="1771" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1770" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1770" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1770">
+        <v>23</v>
+      </c>
+      <c r="G1770" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1770" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1770">
+        <v>10</v>
+      </c>
+      <c r="J1770" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1770">
+        <v>1</v>
+      </c>
+      <c r="L1770" t="s">
+        <v>99</v>
+      </c>
+      <c r="M1770" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1770" t="s">
+        <v>504</v>
+      </c>
+      <c r="R1770" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="1771" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1771">
         <v>1772</v>
       </c>
-    </row>
-    <row r="1772" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1771" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1771" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1771">
+        <v>23</v>
+      </c>
+      <c r="G1771" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1771" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1771">
+        <v>4</v>
+      </c>
+      <c r="J1771" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1771">
+        <v>1</v>
+      </c>
+      <c r="L1771" t="s">
+        <v>99</v>
+      </c>
+      <c r="M1771" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1771" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="1772" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1772">
         <v>1773</v>
       </c>
-    </row>
-    <row r="1773" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1772" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1772" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1772">
+        <v>23</v>
+      </c>
+      <c r="G1772" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1772" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1772">
+        <v>9</v>
+      </c>
+      <c r="J1772" t="s">
+        <v>380</v>
+      </c>
+      <c r="K1772">
+        <v>1</v>
+      </c>
+      <c r="L1772" t="s">
+        <v>148</v>
+      </c>
+      <c r="M1772" t="s">
+        <v>505</v>
+      </c>
+      <c r="P1772" t="s">
+        <v>388</v>
+      </c>
+      <c r="Q1772" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="1773" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1773">
         <v>1774</v>
       </c>
-    </row>
-    <row r="1774" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1773" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1773" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1773">
+        <v>23</v>
+      </c>
+      <c r="G1773" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1773" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1773">
+        <v>5</v>
+      </c>
+      <c r="J1773" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1773">
+        <v>1</v>
+      </c>
+      <c r="L1773" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1773" t="s">
+        <v>145</v>
+      </c>
+      <c r="P1773" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q1773" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="1774" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1774">
         <v>1775</v>
       </c>
-    </row>
-    <row r="1775" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1774" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1774" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1774">
+        <v>23</v>
+      </c>
+      <c r="G1774" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1774" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1774">
+        <v>5</v>
+      </c>
+      <c r="J1774" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1774">
+        <v>1</v>
+      </c>
+      <c r="L1774" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="1775" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1775">
         <v>1776</v>
       </c>
-    </row>
-    <row r="1776" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1775" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1775" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1775">
+        <v>23</v>
+      </c>
+      <c r="G1775" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1775" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1775">
+        <v>5</v>
+      </c>
+      <c r="J1775" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1775">
+        <v>2</v>
+      </c>
+      <c r="L1775" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="1776" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1776">
         <v>1777</v>
       </c>
-    </row>
-    <row r="1777" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1776" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1776" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1776">
+        <v>23</v>
+      </c>
+      <c r="G1776" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1776" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1776">
+        <v>7</v>
+      </c>
+      <c r="J1776" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1776">
+        <v>1</v>
+      </c>
+      <c r="L1776" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1777" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1777">
         <v>1778</v>
       </c>
-    </row>
-    <row r="1778" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1777" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1777" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1777">
+        <v>23</v>
+      </c>
+      <c r="G1777" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1777" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1777">
+        <v>7</v>
+      </c>
+      <c r="J1777" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1777">
+        <v>1</v>
+      </c>
+      <c r="L1777" t="s">
+        <v>251</v>
+      </c>
+      <c r="M1777" t="s">
+        <v>252</v>
+      </c>
+      <c r="P1777" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="1778" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1778">
         <v>1779</v>
       </c>
-    </row>
-    <row r="1779" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1778" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1778" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1778">
+        <v>23</v>
+      </c>
+      <c r="G1778" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1778" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1778">
+        <v>7</v>
+      </c>
+      <c r="J1778" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1778">
+        <v>1</v>
+      </c>
+      <c r="L1778" t="s">
+        <v>148</v>
+      </c>
+      <c r="R1778" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="1779" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1779">
         <v>1780</v>
       </c>
-    </row>
-    <row r="1780" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1779" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1779" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1779">
+        <v>23</v>
+      </c>
+      <c r="G1779" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1779" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1779">
+        <v>7</v>
+      </c>
+      <c r="J1779" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1779">
+        <v>1</v>
+      </c>
+      <c r="L1779" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1779" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="1780" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1780">
         <v>1781</v>
       </c>
-    </row>
-    <row r="1781" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1780" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1780" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1780">
+        <v>23</v>
+      </c>
+      <c r="G1780" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1780" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1780">
+        <v>4</v>
+      </c>
+      <c r="J1780" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1780">
+        <v>1</v>
+      </c>
+      <c r="L1780" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="1781" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1781">
         <v>1782</v>
       </c>
-    </row>
-    <row r="1782" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1781" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1781" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1781">
+        <v>23</v>
+      </c>
+      <c r="G1781" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1781" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1781">
+        <v>4</v>
+      </c>
+      <c r="J1781" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1781">
+        <v>1</v>
+      </c>
+      <c r="L1781" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="1782" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1782">
         <v>1783</v>
       </c>
-    </row>
-    <row r="1783" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D1782" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1782" t="s">
+        <v>492</v>
+      </c>
+      <c r="F1782">
+        <v>23</v>
+      </c>
+      <c r="G1782" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1782" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1782">
+        <v>4</v>
+      </c>
+      <c r="J1782" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1782">
+        <v>1</v>
+      </c>
+      <c r="L1782" t="s">
+        <v>148</v>
+      </c>
+      <c r="M1782" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="1783" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1783">
         <v>1784</v>
       </c>
     </row>
-    <row r="1784" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1784" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1784">
         <v>1785</v>
       </c>
     </row>
-    <row r="1785" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1785" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1785">
         <v>1786</v>
       </c>
     </row>
-    <row r="1786" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1786" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1786">
         <v>1787</v>
       </c>
     </row>
-    <row r="1787" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1787" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1787">
         <v>1788</v>
       </c>
     </row>
-    <row r="1788" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1788" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1788">
         <v>1789</v>
       </c>
     </row>
-    <row r="1789" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1789" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1789">
         <v>1790</v>
       </c>
     </row>
-    <row r="1790" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1790" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1790">
         <v>1791</v>
       </c>
     </row>
-    <row r="1791" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1791" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1791">
         <v>1792</v>
       </c>
     </row>
-    <row r="1792" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1792" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1792">
         <v>1793</v>
       </c>

</xml_diff>